<commit_message>
Lagt till Ring och Shield som items, samt olika equipment types och item sizes.
</commit_message>
<xml_diff>
--- a/Documents/Item_Beslutstabell.xlsx
+++ b/Documents/Item_Beslutstabell.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jon/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jon/Programmering/GitHub/INTE-spelet/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{BFA98460-027C-0E4F-A343-50B50619CEA4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{335811F5-1DBE-8F49-870A-75835ADEF41C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16280" xr2:uid="{E0BCFC50-83D9-EA44-9C0D-3790F3676A66}"/>
+    <workbookView xWindow="380" yWindow="500" windowWidth="28040" windowHeight="16280" activeTab="1" xr2:uid="{E0BCFC50-83D9-EA44-9C0D-3790F3676A66}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
+    <sheet name="Blad2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="202" uniqueCount="35">
   <si>
     <t>Egg</t>
   </si>
@@ -115,13 +116,37 @@
   </si>
   <si>
     <t>Beslutstabell för itemklassen</t>
+  </si>
+  <si>
+    <t>Shield</t>
+  </si>
+  <si>
+    <t>Ring</t>
+  </si>
+  <si>
+    <t>R10</t>
+  </si>
+  <si>
+    <t>R11</t>
+  </si>
+  <si>
+    <t>R12</t>
+  </si>
+  <si>
+    <t>R13</t>
+  </si>
+  <si>
+    <t>R14</t>
+  </si>
+  <si>
+    <t>R15</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -160,13 +185,53 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -187,10 +252,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -202,8 +269,22 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="1" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Bra" xfId="1" builtinId="26"/>
+    <cellStyle name="Dålig" xfId="2" builtinId="27"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -518,7 +599,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D179D41E-B820-BF4A-8B6B-B45F7BCF359C}">
   <dimension ref="A1:J16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -784,4 +867,418 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B8D36C45-6B50-6F45-91E3-B01906E65ED0}">
+  <dimension ref="A1:P16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:16" ht="26" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A5" s="17"/>
+      <c r="B5" s="17" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="H5" s="17" t="s">
+        <v>21</v>
+      </c>
+      <c r="I5" s="17" t="s">
+        <v>22</v>
+      </c>
+      <c r="J5" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" s="22" t="s">
+        <v>29</v>
+      </c>
+      <c r="L5" s="22" t="s">
+        <v>30</v>
+      </c>
+      <c r="M5" s="22" t="s">
+        <v>31</v>
+      </c>
+      <c r="N5" s="17" t="s">
+        <v>32</v>
+      </c>
+      <c r="O5" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="P5" s="17" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A6" s="18" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>3</v>
+      </c>
+      <c r="E6" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="G6" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="I6" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>0</v>
+      </c>
+      <c r="K6" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="L6" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="M6" s="15" t="s">
+        <v>27</v>
+      </c>
+      <c r="N6" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="O6" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="P6" s="12" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A7" s="19" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="E7" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="I7" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="J7" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="K7" s="16" t="s">
+        <v>4</v>
+      </c>
+      <c r="L7" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="M7" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="N7" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="O7" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="P7" s="13" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A8" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="E8" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="G8" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="I8" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="J8" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="K8" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="L8" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="M8" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="N8" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="O8" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="P8" s="12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" ht="21" x14ac:dyDescent="0.25">
+      <c r="A11" s="7" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A13" s="14"/>
+      <c r="B13" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="C13" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="E13" s="17" t="s">
+        <v>18</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>19</v>
+      </c>
+      <c r="G13" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H13" s="22" t="s">
+        <v>21</v>
+      </c>
+      <c r="I13" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="J13" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="K13" s="17" t="s">
+        <v>29</v>
+      </c>
+      <c r="L13" s="17" t="s">
+        <v>30</v>
+      </c>
+      <c r="M13" s="17" t="s">
+        <v>31</v>
+      </c>
+      <c r="N13" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="O13" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="P13" s="22" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A14" s="20" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>2</v>
+      </c>
+      <c r="H14" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="I14" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="J14" s="15" t="s">
+        <v>0</v>
+      </c>
+      <c r="K14" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="L14" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="M14" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="N14" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="O14" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="P14" s="15" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A15" s="21" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="D15" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="H15" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="I15" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="J15" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="K15" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="L15" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="M15" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="N15" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="O15" s="16" t="s">
+        <v>13</v>
+      </c>
+      <c r="P15" s="16" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="A16" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="C16" s="14"/>
+      <c r="D16" s="14"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="G16" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="I16" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="J16" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="K16" s="12" t="s">
+        <v>7</v>
+      </c>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
+      <c r="N16" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="O16" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="P16" s="15" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>